<commit_message>
update sidebar dan halaman evaluasi
</commit_message>
<xml_diff>
--- a/penilaian-ZI.xlsx
+++ b/penilaian-ZI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\project\sibekisar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7950AAE-C392-4B06-B95D-255E4C44910D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFF3CD2-0BC7-4CE9-8D97-107C3DB945B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{81ABB71F-C48B-4169-A963-AC8D91DB89DC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{81ABB71F-C48B-4169-A963-AC8D91DB89DC}"/>
   </bookViews>
   <sheets>
     <sheet name="RB General" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2683" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2721" uniqueCount="740">
   <si>
     <t>Indikator</t>
   </si>
@@ -2221,13 +2221,52 @@
   </si>
   <si>
     <t>nilai_input</t>
+  </si>
+  <si>
+    <t>Indikator untuk aspek 1</t>
+  </si>
+  <si>
+    <t>id_aspek</t>
+  </si>
+  <si>
+    <t>periode</t>
+  </si>
+  <si>
+    <t>jml_periode</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>is_aktif</t>
+  </si>
+  <si>
+    <t>opd</t>
+  </si>
+  <si>
+    <t>C020250101</t>
+  </si>
+  <si>
+    <t>C020250102</t>
+  </si>
+  <si>
+    <t>C020250104</t>
+  </si>
+  <si>
+    <t>C0202501</t>
+  </si>
+  <si>
+    <t>insert into m_indikator (id_indikator,indikator,id_aspek,bobot,nilai_maks,periode,jml_periode,opd_pengampu,id_opd,tag,keterangan,is_aktif) values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2252,8 +2291,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2269,6 +2314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2337,7 +2388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2406,6 +2457,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3652,10 +3708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D07F0DB-ECA4-40B5-85F8-3C2ACB2284B0}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35:M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4394,7 +4450,223 @@
         <v>7</v>
       </c>
     </row>
+    <row r="34" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="27" t="s">
+        <v>727</v>
+      </c>
+      <c r="D34" s="29"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>728</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>729</v>
+      </c>
+      <c r="G35" t="s">
+        <v>730</v>
+      </c>
+      <c r="H35" t="s">
+        <v>712</v>
+      </c>
+      <c r="I35" t="s">
+        <v>713</v>
+      </c>
+      <c r="J35" t="s">
+        <v>731</v>
+      </c>
+      <c r="K35" t="s">
+        <v>732</v>
+      </c>
+      <c r="L35" t="s">
+        <v>733</v>
+      </c>
+      <c r="M35" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>735</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>738</v>
+      </c>
+      <c r="D36" s="17">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>715</v>
+      </c>
+      <c r="I36">
+        <v>55</v>
+      </c>
+      <c r="J36" t="s">
+        <v>734</v>
+      </c>
+      <c r="K36" t="s">
+        <v>715</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36" t="str">
+        <f>"('"&amp;A36&amp;"', '"&amp;B36&amp;"', '"&amp;C36&amp;"', "&amp;D36&amp;", "&amp;E36&amp;", "&amp;F36&amp;", "&amp;G36&amp;", '"&amp;H36&amp;"', "&amp;I36&amp;", '"&amp;J36&amp;"', '"&amp;K36&amp;"', "&amp;L36&amp;"),"</f>
+        <v>('C020250101', 'Rencana Aksi Pembangunan RB General', 'C0202501', 3, 100, 1, 1, 'Biro Organisasi', 55, 'opd', 'Biro Organisasi', 1),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>736</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>738</v>
+      </c>
+      <c r="D37" s="17">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>722</v>
+      </c>
+      <c r="I37">
+        <v>39</v>
+      </c>
+      <c r="J37" t="s">
+        <v>734</v>
+      </c>
+      <c r="K37" t="s">
+        <v>722</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" ref="M37:M39" si="1">"('"&amp;A37&amp;"', '"&amp;B37&amp;"', '"&amp;C37&amp;"', "&amp;D37&amp;", "&amp;E37&amp;", "&amp;F37&amp;", "&amp;G37&amp;", '"&amp;H37&amp;"', "&amp;I37&amp;", '"&amp;J37&amp;"', '"&amp;K37&amp;"', "&amp;L37&amp;"),"</f>
+        <v>('C020250102', 'Tingkat Implementasi Rencana Aksi RB General', 'C0202501', 3, 100, 1, 1, 'Inspektorat', 39, 'opd', 'Inspektorat', 1),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>738</v>
+      </c>
+      <c r="D38" s="17">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>715</v>
+      </c>
+      <c r="I38">
+        <v>55</v>
+      </c>
+      <c r="J38" t="s">
+        <v>734</v>
+      </c>
+      <c r="K38" t="s">
+        <v>715</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="1"/>
+        <v>('C020250103', 'Capaian IKU', 'C0202501', 2, 100, 1, 1, 'Biro Organisasi', 55, 'opd', 'Biro Organisasi', 1),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>737</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>738</v>
+      </c>
+      <c r="D39" s="17">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>100</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>715</v>
+      </c>
+      <c r="I39">
+        <v>55</v>
+      </c>
+      <c r="J39" t="s">
+        <v>734</v>
+      </c>
+      <c r="K39" t="s">
+        <v>715</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="1"/>
+        <v>('C020250104', 'Kinerja Agen Perubahan', 'C0202501', 2, 100, 1, 1, 'Biro Organisasi', 55, 'opd', 'Biro Organisasi', 1),</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -4405,7 +4677,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V14560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C394" sqref="C394"/>
     </sheetView>
   </sheetViews>
@@ -26705,11 +26977,11 @@
         <v>3</v>
       </c>
       <c r="I578" s="15">
-        <f t="shared" ref="I578:I641" si="18">(G578/F578)*H578</f>
+        <f t="shared" ref="I578:I612" si="18">(G578/F578)*H578</f>
         <v>0.60000000000000009</v>
       </c>
       <c r="J578" t="str">
-        <f t="shared" ref="J578:J641" si="19">"update evaluasi set tahun = "&amp;E578&amp;", nilai_maks = "&amp;F578&amp;", nilai_input="&amp;G578&amp;", bobot = "&amp;H578&amp;", nilai_akhir = "&amp;I578&amp;", id_indikator = '"&amp;C578&amp;"' where id_evaluasi = '"&amp;A578&amp;"';"</f>
+        <f t="shared" ref="J578:J612" si="19">"update evaluasi set tahun = "&amp;E578&amp;", nilai_maks = "&amp;F578&amp;", nilai_input="&amp;G578&amp;", bobot = "&amp;H578&amp;", nilai_akhir = "&amp;I578&amp;", id_indikator = '"&amp;C578&amp;"' where id_evaluasi = '"&amp;A578&amp;"';"</f>
         <v>update evaluasi set tahun = 1, nilai_maks = 5, nilai_input=1, bobot = 3, nilai_akhir = 0.6, id_indikator = 'C020250229' where id_evaluasi = '20250030_C020250605';</v>
       </c>
     </row>

</xml_diff>